<commit_message>
MCQ excel file added
</commit_message>
<xml_diff>
--- a/Core Java-mcqs .xlsx
+++ b/Core Java-mcqs .xlsx
@@ -11963,7 +11963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N676"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -11974,7 +11974,7 @@
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75">
@@ -12060,8 +12060,13 @@
         <v>1</v>
       </c>
       <c r="N2" s="2" t="str">
-        <f xml:space="preserve"> "$x=Question::create(['"&amp;$A$1&amp;"'=&gt;"&amp;A2</f>
-        <v>$x=Question::create(['question_level_id'=&gt;1</v>
+        <f xml:space="preserve"> "$x=Question::create(['"&amp;$A$1&amp;"'=&gt;"&amp;A2&amp;",'"&amp;$B$1&amp;"'=&gt;"&amp;B2&amp;",'"&amp;$C$1&amp;"'=&gt;"&amp;C2&amp;",'"&amp;$D$1&amp;"'=&gt;'"&amp;D2&amp;"']); Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'"&amp;E2&amp;"','is_answer'=&gt;"&amp;J2&amp;"]);  Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'"&amp;F2&amp;"','is_answer'=&gt;"&amp;K2&amp;"]);  Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'"&amp;G2&amp;"','is_answer'=&gt;"&amp;L2&amp;"]); Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'"&amp;H2&amp;"','is_answer'=&gt;"&amp;M2&amp;"]); "</f>
+        <v xml:space="preserve">$x=Question::create(['question_level_id'=&gt;1,'chapter_id'=&gt;1,'question_type_id'=&gt;1,'question'=&gt;'Consider the following code and choose the correct option:
+class X { int x; X(int x){x=2;}}
+class Y extends X{ Y(){} void displayX(){
+System.out.print(x);}
+public static void main(String args[]){
+ new Y().displayX();}}']); Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'Compiles and display 2','is_answer'=&gt;0]);  Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'Compiles and runs without any output','is_answer'=&gt;0]);  Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'Compiles and display 0','is_answer'=&gt;0]); Option::create(['question_id'=&gt;$x-&gt;id,'option'=&gt;'Compilation error','is_answer'=&gt;1]); </v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="120">

</xml_diff>